<commit_message>
Updated graphs - added axis markups and created graphs.png
</commit_message>
<xml_diff>
--- a/sorting_algorithms_time_comparison_graphs.xlsx
+++ b/sorting_algorithms_time_comparison_graphs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mateusz\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\mwasilew\sem2\AISDI\lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A56187-C77A-418E-84D4-2B10CE3545AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FAECD6D-0DFB-4225-886B-78DE45EFB227}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{21F5CC27-C301-4B5E-AC40-0E9E5AD197D1}"/>
   </bookViews>
@@ -559,6 +559,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>liczba posortowanych znaków</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -607,7 +662,7 @@
         <c:axId val="1845135296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1"/>
+          <c:max val="3"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -625,6 +680,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>czas[s]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -896,7 +1006,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7E32-418A-8D22-2F251EEAB1A5}"/>
+              <c16:uniqueId val="{00000001-79DA-472A-9286-214A57AB2723}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -974,7 +1084,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-7E32-418A-8D22-2F251EEAB1A5}"/>
+              <c16:uniqueId val="{00000002-79DA-472A-9286-214A57AB2723}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1052,7 +1162,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-7E32-418A-8D22-2F251EEAB1A5}"/>
+              <c16:uniqueId val="{00000003-79DA-472A-9286-214A57AB2723}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1207,7 +1317,7 @@
                 <c:smooth val="0"/>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000000-7E32-418A-8D22-2F251EEAB1A5}"/>
+                    <c16:uniqueId val="{00000000-79DA-472A-9286-214A57AB2723}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -1222,6 +1332,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>liczba posortowanych znaków</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1270,7 +1435,7 @@
         <c:axId val="1845135296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="5.000000000000001E-2"/>
+          <c:max val="3.0000000000000006E-2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1288,6 +1453,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>czas[s]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2559,22 +2779,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>616323</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>627529</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>56029</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>1277470</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>78442</xdr:rowOff>
+      <xdr:colOff>1288676</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Wykres 3">
+        <xdr:cNvPr id="5" name="Wykres 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D6AD298-70F3-4C91-9DFF-4810895C86C0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E38AE158-D78F-4485-AD42-05AC479000F3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2896,8 +3116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9D562D4-F83A-4305-BF30-B4327E178227}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L47" sqref="L47"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V21" sqref="V21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>